<commit_message>
correction calcul et nouvelle fichier
</commit_message>
<xml_diff>
--- a/trg_simu.xlsx
+++ b/trg_simu.xlsx
@@ -5,8 +5,8 @@
   <sheets>
     <sheet state="visible" name="main" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="data_2024" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="data_2022" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="data_2023" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="data_2023" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="data_2022" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="calcul_prime" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
@@ -87,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -106,12 +106,16 @@
       <name val="Aptos Narrow"/>
     </font>
     <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -130,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -142,9 +146,13 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2593,7 +2601,7 @@
       <c r="G11" s="1">
         <v>74.244</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="4">
         <v>0.0</v>
       </c>
     </row>
@@ -2677,28 +2685,28 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>81.9</v>
+        <v>84.014</v>
       </c>
       <c r="D2" s="1">
         <v>140.0</v>
       </c>
       <c r="E2" s="1">
-        <v>80.41</v>
+        <v>79.02975853612529</v>
       </c>
       <c r="F2" s="1">
         <v>120.0</v>
       </c>
       <c r="G2" s="1">
-        <v>74.958</v>
+        <v>78.24</v>
       </c>
       <c r="H2" s="1">
-        <v>60.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="3">
@@ -2707,22 +2715,22 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>82.41011904761905</v>
+        <v>80.165</v>
       </c>
       <c r="D3" s="1">
         <v>140.0</v>
       </c>
       <c r="E3" s="1">
-        <v>77.831</v>
+        <v>82.01</v>
       </c>
       <c r="F3" s="1">
-        <v>100.0</v>
+        <v>140.0</v>
       </c>
       <c r="G3" s="1">
-        <v>77.91</v>
+        <v>79.9722132034632</v>
       </c>
       <c r="H3" s="1">
-        <v>100.0</v>
+        <v>140.0</v>
       </c>
     </row>
     <row r="4">
@@ -2731,19 +2739,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>84.34</v>
+        <v>82.035</v>
       </c>
       <c r="D4" s="1">
         <v>140.0</v>
       </c>
       <c r="E4" s="1">
-        <v>80.22519335974346</v>
+        <v>79.41695906432749</v>
       </c>
       <c r="F4" s="1">
         <v>120.0</v>
       </c>
       <c r="G4" s="1">
-        <v>85.399</v>
+        <v>81.959</v>
       </c>
       <c r="H4" s="1">
         <v>140.0</v>
@@ -2755,19 +2763,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>81.87</v>
+        <v>86.56</v>
       </c>
       <c r="D5" s="1">
         <v>140.0</v>
       </c>
       <c r="E5" s="1">
-        <v>80.622</v>
+        <v>80.804</v>
       </c>
       <c r="F5" s="1">
         <v>140.0</v>
       </c>
       <c r="G5" s="1">
-        <v>79.211</v>
+        <v>79.219</v>
       </c>
       <c r="H5" s="1">
         <v>120.0</v>
@@ -2779,22 +2787,22 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>84.864</v>
+        <v>87.674</v>
       </c>
       <c r="D6" s="1">
         <v>140.0</v>
       </c>
       <c r="E6" s="1">
-        <v>82.046</v>
+        <v>82.228</v>
       </c>
       <c r="F6" s="1">
         <v>140.0</v>
       </c>
       <c r="G6" s="1">
-        <v>82.763</v>
+        <v>78.249</v>
       </c>
       <c r="H6" s="1">
-        <v>140.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="7">
@@ -2803,19 +2811,19 @@
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>82.66266666666665</v>
+        <v>89.405</v>
       </c>
       <c r="D7" s="1">
         <v>140.0</v>
       </c>
       <c r="E7" s="1">
-        <v>80.135</v>
+        <v>76.824</v>
       </c>
       <c r="F7" s="1">
-        <v>120.0</v>
+        <v>80.0</v>
       </c>
       <c r="G7" s="1">
-        <v>80.92809343434344</v>
+        <v>79.893</v>
       </c>
       <c r="H7" s="1">
         <v>140.0</v>
@@ -2827,22 +2835,22 @@
         <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>82.77</v>
+        <v>87.307</v>
       </c>
       <c r="D8" s="1">
         <v>140.0</v>
       </c>
       <c r="E8" s="1">
-        <v>79.042</v>
+        <v>80.676</v>
       </c>
       <c r="F8" s="1">
-        <v>120.0</v>
+        <v>140.0</v>
       </c>
       <c r="G8" s="1">
-        <v>81.1</v>
+        <v>74.197</v>
       </c>
       <c r="H8" s="1">
-        <v>140.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -2851,22 +2859,22 @@
         <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>84.561</v>
+        <v>84.99893518518519</v>
       </c>
       <c r="D9" s="1">
         <v>140.0</v>
       </c>
       <c r="E9" s="1">
-        <v>82.168</v>
+        <v>77.17</v>
       </c>
       <c r="F9" s="1">
-        <v>140.0</v>
+        <v>80.0</v>
       </c>
       <c r="G9" s="1">
-        <v>78.968</v>
+        <v>74.888</v>
       </c>
       <c r="H9" s="1">
-        <v>120.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="10">
@@ -2875,22 +2883,22 @@
         <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>82.58</v>
+        <v>84.575</v>
       </c>
       <c r="D10" s="1">
         <v>140.0</v>
       </c>
       <c r="E10" s="1">
-        <v>82.62</v>
+        <v>79.86</v>
       </c>
       <c r="F10" s="1">
-        <v>140.0</v>
+        <v>120.0</v>
       </c>
       <c r="G10" s="1">
-        <v>79.604</v>
+        <v>73.271</v>
       </c>
       <c r="H10" s="1">
-        <v>140.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -2899,22 +2907,22 @@
         <v>13</v>
       </c>
       <c r="C11" s="1">
-        <v>76.878</v>
+        <v>88.918</v>
       </c>
       <c r="D11" s="1">
         <v>140.0</v>
       </c>
       <c r="E11" s="1">
-        <v>76.6263401559454</v>
+        <v>81.89982201881514</v>
       </c>
       <c r="F11" s="1">
-        <v>80.0</v>
+        <v>140.0</v>
       </c>
       <c r="G11" s="1">
-        <v>70.743</v>
+        <v>77.146</v>
       </c>
       <c r="H11" s="1">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="12">
@@ -2923,22 +2931,22 @@
         <v>14</v>
       </c>
       <c r="C12" s="1">
-        <v>79.647</v>
+        <v>85.836</v>
       </c>
       <c r="D12" s="1">
         <v>140.0</v>
       </c>
       <c r="E12" s="1">
-        <v>77.711</v>
+        <v>77.29031713900135</v>
       </c>
       <c r="F12" s="1">
-        <v>100.0</v>
+        <v>80.0</v>
       </c>
       <c r="G12" s="1">
-        <v>76.539</v>
+        <v>73.17004545454544</v>
       </c>
       <c r="H12" s="1">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -2947,22 +2955,22 @@
         <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>83.692</v>
+        <v>91.3480107526882</v>
       </c>
       <c r="D13" s="1">
         <v>140.0</v>
       </c>
       <c r="E13" s="1">
-        <v>80.926</v>
+        <v>79.776</v>
       </c>
       <c r="F13" s="1">
-        <v>140.0</v>
+        <v>120.0</v>
       </c>
       <c r="G13" s="1">
-        <v>78.554</v>
+        <v>77.42537878787878</v>
       </c>
       <c r="H13" s="1">
-        <v>120.0</v>
+        <v>100.0</v>
       </c>
     </row>
   </sheetData>
@@ -2981,7 +2989,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="5"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -2997,28 +3005,28 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>2023.0</v>
+        <v>2022.0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>84.014</v>
+        <v>81.9</v>
       </c>
       <c r="D2" s="1">
         <v>140.0</v>
       </c>
       <c r="E2" s="1">
-        <v>79.02975853612529</v>
+        <v>80.41</v>
       </c>
       <c r="F2" s="1">
         <v>120.0</v>
       </c>
       <c r="G2" s="1">
-        <v>78.24</v>
+        <v>74.958</v>
       </c>
       <c r="H2" s="1">
-        <v>120.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="3">
@@ -3027,22 +3035,22 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>80.165</v>
+        <v>82.41011904761905</v>
       </c>
       <c r="D3" s="1">
         <v>140.0</v>
       </c>
       <c r="E3" s="1">
-        <v>82.01</v>
+        <v>77.831</v>
       </c>
       <c r="F3" s="1">
-        <v>140.0</v>
+        <v>100.0</v>
       </c>
       <c r="G3" s="1">
-        <v>79.9722132034632</v>
+        <v>77.91</v>
       </c>
       <c r="H3" s="1">
-        <v>140.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="4">
@@ -3051,19 +3059,19 @@
         <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>82.035</v>
+        <v>84.34</v>
       </c>
       <c r="D4" s="1">
         <v>140.0</v>
       </c>
       <c r="E4" s="1">
-        <v>79.41695906432749</v>
+        <v>80.22519335974346</v>
       </c>
       <c r="F4" s="1">
         <v>120.0</v>
       </c>
       <c r="G4" s="1">
-        <v>81.959</v>
+        <v>85.399</v>
       </c>
       <c r="H4" s="1">
         <v>140.0</v>
@@ -3075,19 +3083,19 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>86.56</v>
+        <v>81.87</v>
       </c>
       <c r="D5" s="1">
         <v>140.0</v>
       </c>
       <c r="E5" s="1">
-        <v>80.804</v>
+        <v>80.622</v>
       </c>
       <c r="F5" s="1">
         <v>140.0</v>
       </c>
       <c r="G5" s="1">
-        <v>79.219</v>
+        <v>79.211</v>
       </c>
       <c r="H5" s="1">
         <v>120.0</v>
@@ -3099,22 +3107,22 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>87.674</v>
+        <v>84.864</v>
       </c>
       <c r="D6" s="1">
         <v>140.0</v>
       </c>
       <c r="E6" s="1">
-        <v>82.228</v>
+        <v>82.046</v>
       </c>
       <c r="F6" s="1">
         <v>140.0</v>
       </c>
       <c r="G6" s="1">
-        <v>78.249</v>
+        <v>82.763</v>
       </c>
       <c r="H6" s="1">
-        <v>120.0</v>
+        <v>140.0</v>
       </c>
     </row>
     <row r="7">
@@ -3123,19 +3131,19 @@
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>89.405</v>
+        <v>82.66266666666665</v>
       </c>
       <c r="D7" s="1">
         <v>140.0</v>
       </c>
       <c r="E7" s="1">
-        <v>76.824</v>
+        <v>80.135</v>
       </c>
       <c r="F7" s="1">
-        <v>80.0</v>
+        <v>120.0</v>
       </c>
       <c r="G7" s="1">
-        <v>79.893</v>
+        <v>80.92809343434344</v>
       </c>
       <c r="H7" s="1">
         <v>140.0</v>
@@ -3147,22 +3155,22 @@
         <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>87.307</v>
+        <v>82.77</v>
       </c>
       <c r="D8" s="1">
         <v>140.0</v>
       </c>
       <c r="E8" s="1">
-        <v>80.676</v>
+        <v>79.042</v>
       </c>
       <c r="F8" s="1">
-        <v>140.0</v>
+        <v>120.0</v>
       </c>
       <c r="G8" s="1">
-        <v>74.197</v>
+        <v>81.1</v>
       </c>
       <c r="H8" s="1">
-        <v>0.0</v>
+        <v>140.0</v>
       </c>
     </row>
     <row r="9">
@@ -3171,22 +3179,22 @@
         <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>84.99893518518519</v>
+        <v>84.561</v>
       </c>
       <c r="D9" s="1">
         <v>140.0</v>
       </c>
       <c r="E9" s="1">
-        <v>77.17</v>
+        <v>82.168</v>
       </c>
       <c r="F9" s="1">
-        <v>80.0</v>
+        <v>140.0</v>
       </c>
       <c r="G9" s="1">
-        <v>74.888</v>
+        <v>78.968</v>
       </c>
       <c r="H9" s="1">
-        <v>60.0</v>
+        <v>120.0</v>
       </c>
     </row>
     <row r="10">
@@ -3195,22 +3203,22 @@
         <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>84.575</v>
+        <v>82.58</v>
       </c>
       <c r="D10" s="1">
         <v>140.0</v>
       </c>
       <c r="E10" s="1">
-        <v>79.86</v>
+        <v>82.62</v>
       </c>
       <c r="F10" s="1">
-        <v>120.0</v>
+        <v>140.0</v>
       </c>
       <c r="G10" s="1">
-        <v>73.271</v>
+        <v>79.604</v>
       </c>
       <c r="H10" s="1">
-        <v>0.0</v>
+        <v>140.0</v>
       </c>
     </row>
     <row r="11">
@@ -3219,22 +3227,22 @@
         <v>13</v>
       </c>
       <c r="C11" s="1">
-        <v>88.918</v>
+        <v>76.878</v>
       </c>
       <c r="D11" s="1">
         <v>140.0</v>
       </c>
       <c r="E11" s="1">
-        <v>81.89982201881514</v>
+        <v>76.6263401559454</v>
       </c>
       <c r="F11" s="1">
-        <v>140.0</v>
+        <v>80.0</v>
       </c>
       <c r="G11" s="1">
-        <v>77.146</v>
+        <v>70.743</v>
       </c>
       <c r="H11" s="1">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
@@ -3243,22 +3251,22 @@
         <v>14</v>
       </c>
       <c r="C12" s="1">
-        <v>85.836</v>
+        <v>79.647</v>
       </c>
       <c r="D12" s="1">
         <v>140.0</v>
       </c>
       <c r="E12" s="1">
-        <v>77.29031713900135</v>
+        <v>77.711</v>
       </c>
       <c r="F12" s="1">
-        <v>80.0</v>
+        <v>100.0</v>
       </c>
       <c r="G12" s="1">
-        <v>73.17004545454544</v>
+        <v>76.539</v>
       </c>
       <c r="H12" s="1">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
     </row>
     <row r="13">
@@ -3267,22 +3275,22 @@
         <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>91.3480107526882</v>
+        <v>83.692</v>
       </c>
       <c r="D13" s="1">
         <v>140.0</v>
       </c>
       <c r="E13" s="1">
-        <v>79.776</v>
+        <v>80.926</v>
       </c>
       <c r="F13" s="1">
-        <v>120.0</v>
+        <v>140.0</v>
       </c>
       <c r="G13" s="1">
-        <v>77.42537878787878</v>
+        <v>78.554</v>
       </c>
       <c r="H13" s="1">
-        <v>100.0</v>
+        <v>120.0</v>
       </c>
     </row>
   </sheetData>
@@ -3301,122 +3309,122 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4">
+      <c r="A2" s="6">
         <v>71.0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="6">
         <v>60.0</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
         <v>75.0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>60.0</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="6">
         <v>74.5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="6">
         <v>60.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4">
+      <c r="A3" s="6">
         <v>72.0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="6">
         <v>80.0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="6">
         <v>76.0</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6">
         <v>80.0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="6">
         <v>75.5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="6">
         <v>80.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
+      <c r="A4" s="6">
         <v>73.0</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="6">
         <v>100.0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="6">
         <v>77.5</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="6">
         <v>100.0</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="6">
         <v>76.5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="6">
         <v>100.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>74.0</v>
       </c>
-      <c r="B5" s="4">
-        <v>120.0</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="6">
+        <v>120.0</v>
+      </c>
+      <c r="C5" s="6">
         <v>78.5</v>
       </c>
-      <c r="D5" s="4">
-        <v>120.0</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="D5" s="6">
+        <v>120.0</v>
+      </c>
+      <c r="E5" s="6">
         <v>78.0</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="6">
         <v>120.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>75.0</v>
       </c>
-      <c r="B6" s="4">
-        <v>140.0</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="6">
+        <v>140.0</v>
+      </c>
+      <c r="C6" s="6">
         <v>80.5</v>
       </c>
-      <c r="D6" s="4">
-        <v>140.0</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D6" s="6">
+        <v>140.0</v>
+      </c>
+      <c r="E6" s="6">
         <v>79.5</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="6">
         <v>140.0</v>
       </c>
     </row>

</xml_diff>